<commit_message>
update. Got rid of Conda.
</commit_message>
<xml_diff>
--- a/FinalOutput-By_Ticker.xlsx
+++ b/FinalOutput-By_Ticker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="298">
   <si>
     <t>dollarsTradedTodayApprox</t>
   </si>
@@ -34,438 +34,426 @@
     <t>ZBRA</t>
   </si>
   <si>
+    <t>GMS</t>
+  </si>
+  <si>
+    <t>ACAD</t>
+  </si>
+  <si>
+    <t>NCLH</t>
+  </si>
+  <si>
+    <t>BMBL</t>
+  </si>
+  <si>
+    <t>ACMR</t>
+  </si>
+  <si>
+    <t>XLRN</t>
+  </si>
+  <si>
+    <t>DELL</t>
+  </si>
+  <si>
+    <t>AMP</t>
+  </si>
+  <si>
+    <t>OXY</t>
+  </si>
+  <si>
+    <t>AVAV</t>
+  </si>
+  <si>
+    <t>WORK</t>
+  </si>
+  <si>
+    <t>DRI</t>
+  </si>
+  <si>
     <t>CCJ</t>
   </si>
   <si>
-    <t>GMS</t>
-  </si>
-  <si>
-    <t>ACAD</t>
-  </si>
-  <si>
-    <t>NCLH</t>
-  </si>
-  <si>
-    <t>BMBL</t>
-  </si>
-  <si>
-    <t>ACMR</t>
+    <t>RAMP</t>
+  </si>
+  <si>
+    <t>SYY</t>
+  </si>
+  <si>
+    <t>BLD</t>
+  </si>
+  <si>
+    <t>OLLI</t>
+  </si>
+  <si>
+    <t>NLOK</t>
+  </si>
+  <si>
+    <t>BCC</t>
+  </si>
+  <si>
+    <t>BWXT</t>
+  </si>
+  <si>
+    <t>JBLU</t>
+  </si>
+  <si>
+    <t>CIEN</t>
+  </si>
+  <si>
+    <t>LBTYK</t>
+  </si>
+  <si>
+    <t>NNOX</t>
+  </si>
+  <si>
+    <t>HPE</t>
+  </si>
+  <si>
+    <t>YELL</t>
+  </si>
+  <si>
+    <t>CTVA</t>
+  </si>
+  <si>
+    <t>PLAN</t>
+  </si>
+  <si>
+    <t>ATSG</t>
+  </si>
+  <si>
+    <t>CYTK</t>
+  </si>
+  <si>
+    <t>BEPC</t>
+  </si>
+  <si>
+    <t>CCMP</t>
+  </si>
+  <si>
+    <t>AAN</t>
+  </si>
+  <si>
+    <t>BRKR</t>
+  </si>
+  <si>
+    <t>ADT</t>
+  </si>
+  <si>
+    <t>UNFI</t>
+  </si>
+  <si>
+    <t>INMD</t>
+  </si>
+  <si>
+    <t>UTZ</t>
+  </si>
+  <si>
+    <t>PPL</t>
+  </si>
+  <si>
+    <t>MYOV</t>
+  </si>
+  <si>
+    <t>BCEL</t>
+  </si>
+  <si>
+    <t>GPS</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>JBL</t>
+  </si>
+  <si>
+    <t>WMB</t>
+  </si>
+  <si>
+    <t>AQN</t>
+  </si>
+  <si>
+    <t>MTN</t>
+  </si>
+  <si>
+    <t>BCEI</t>
+  </si>
+  <si>
+    <t>WTRG</t>
+  </si>
+  <si>
+    <t>ARDX</t>
   </si>
   <si>
     <t>CHEF</t>
   </si>
   <si>
-    <t>XLRN</t>
-  </si>
-  <si>
-    <t>AMP</t>
+    <t>AQB</t>
+  </si>
+  <si>
+    <t>KKR</t>
+  </si>
+  <si>
+    <t>IBN</t>
+  </si>
+  <si>
+    <t>SONO</t>
+  </si>
+  <si>
+    <t>NEWR</t>
+  </si>
+  <si>
+    <t>ITCI</t>
+  </si>
+  <si>
+    <t>HTZGQ</t>
+  </si>
+  <si>
+    <t>SILV</t>
+  </si>
+  <si>
+    <t>RHP</t>
+  </si>
+  <si>
+    <t>NAV</t>
+  </si>
+  <si>
+    <t>JAZZ</t>
+  </si>
+  <si>
+    <t>WEC</t>
+  </si>
+  <si>
+    <t>EVRG</t>
+  </si>
+  <si>
+    <t>AERI</t>
+  </si>
+  <si>
+    <t>UGI</t>
+  </si>
+  <si>
+    <t>MDLA</t>
+  </si>
+  <si>
+    <t>CVE</t>
+  </si>
+  <si>
+    <t>AGEN</t>
+  </si>
+  <si>
+    <t>IDCC</t>
+  </si>
+  <si>
+    <t>USAC</t>
+  </si>
+  <si>
+    <t>ALGM</t>
+  </si>
+  <si>
+    <t>OSH</t>
+  </si>
+  <si>
+    <t>EPZM</t>
+  </si>
+  <si>
+    <t>TROX</t>
+  </si>
+  <si>
+    <t>NS</t>
+  </si>
+  <si>
+    <t>DCI</t>
+  </si>
+  <si>
+    <t>GPMT</t>
+  </si>
+  <si>
+    <t>BKEP</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>TMDX</t>
+  </si>
+  <si>
+    <t>GNL</t>
   </si>
   <si>
     <t>CARA</t>
   </si>
   <si>
-    <t>CTVA</t>
-  </si>
-  <si>
-    <t>DELL</t>
-  </si>
-  <si>
-    <t>WORK</t>
-  </si>
-  <si>
-    <t>OXY</t>
-  </si>
-  <si>
-    <t>CIEN</t>
-  </si>
-  <si>
-    <t>AVAV</t>
-  </si>
-  <si>
-    <t>DRI</t>
-  </si>
-  <si>
-    <t>RAMP</t>
-  </si>
-  <si>
-    <t>SYY</t>
-  </si>
-  <si>
-    <t>BLD</t>
+    <t>QLYS</t>
+  </si>
+  <si>
+    <t>HAE</t>
+  </si>
+  <si>
+    <t>CAL</t>
+  </si>
+  <si>
+    <t>BRG</t>
+  </si>
+  <si>
+    <t>SMSI</t>
+  </si>
+  <si>
+    <t>KIN</t>
+  </si>
+  <si>
+    <t>SMCI</t>
+  </si>
+  <si>
+    <t>ARAV</t>
+  </si>
+  <si>
+    <t>LCI</t>
+  </si>
+  <si>
+    <t>PLX</t>
+  </si>
+  <si>
+    <t>RBA</t>
+  </si>
+  <si>
+    <t>RADA</t>
+  </si>
+  <si>
+    <t>IEP</t>
+  </si>
+  <si>
+    <t>GRBK</t>
+  </si>
+  <si>
+    <t>BRFS</t>
+  </si>
+  <si>
+    <t>VGR</t>
+  </si>
+  <si>
+    <t>KRMD</t>
+  </si>
+  <si>
+    <t>VOYA</t>
+  </si>
+  <si>
+    <t>CEMI</t>
+  </si>
+  <si>
+    <t>WIFI</t>
+  </si>
+  <si>
+    <t>CRI</t>
+  </si>
+  <si>
+    <t>RCM</t>
+  </si>
+  <si>
+    <t>SUPN</t>
+  </si>
+  <si>
+    <t>QTRX</t>
+  </si>
+  <si>
+    <t>JELD</t>
+  </si>
+  <si>
+    <t>SID</t>
+  </si>
+  <si>
+    <t>IPI</t>
+  </si>
+  <si>
+    <t>STIM</t>
+  </si>
+  <si>
+    <t>CVA</t>
+  </si>
+  <si>
+    <t>HALL</t>
+  </si>
+  <si>
+    <t>SMFG</t>
+  </si>
+  <si>
+    <t>APTX</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>REKR</t>
+  </si>
+  <si>
+    <t>CWK</t>
   </si>
   <si>
     <t>CNR</t>
   </si>
   <si>
-    <t>OLLI</t>
-  </si>
-  <si>
-    <t>NLOK</t>
-  </si>
-  <si>
-    <t>CRI</t>
-  </si>
-  <si>
-    <t>BCC</t>
-  </si>
-  <si>
-    <t>CEMI</t>
-  </si>
-  <si>
-    <t>BWXT</t>
-  </si>
-  <si>
-    <t>CCMP</t>
-  </si>
-  <si>
-    <t>JBLU</t>
-  </si>
-  <si>
-    <t>LBTYK</t>
-  </si>
-  <si>
-    <t>CVE</t>
-  </si>
-  <si>
-    <t>NNOX</t>
-  </si>
-  <si>
-    <t>HPE</t>
-  </si>
-  <si>
-    <t>YELL</t>
-  </si>
-  <si>
-    <t>PLAN</t>
-  </si>
-  <si>
-    <t>CYTK</t>
-  </si>
-  <si>
-    <t>ATSG</t>
-  </si>
-  <si>
-    <t>BEPC</t>
-  </si>
-  <si>
-    <t>CAL</t>
-  </si>
-  <si>
-    <t>AAN</t>
+    <t>MBI</t>
+  </si>
+  <si>
+    <t>MATX</t>
+  </si>
+  <si>
+    <t>UUUU</t>
+  </si>
+  <si>
+    <t>UEC</t>
+  </si>
+  <si>
+    <t>LEAF</t>
+  </si>
+  <si>
+    <t>KYN</t>
+  </si>
+  <si>
+    <t>CNTY</t>
+  </si>
+  <si>
+    <t>FNHC</t>
+  </si>
+  <si>
+    <t>EZPW</t>
+  </si>
+  <si>
+    <t>SBBP</t>
+  </si>
+  <si>
+    <t>EVC</t>
+  </si>
+  <si>
+    <t>ETH</t>
   </si>
   <si>
     <t>CNA</t>
   </si>
   <si>
-    <t>ADT</t>
-  </si>
-  <si>
-    <t>UNFI</t>
-  </si>
-  <si>
-    <t>INMD</t>
-  </si>
-  <si>
-    <t>UTZ</t>
-  </si>
-  <si>
-    <t>PPL</t>
-  </si>
-  <si>
-    <t>BCEL</t>
-  </si>
-  <si>
-    <t>MYOV</t>
-  </si>
-  <si>
-    <t>BCEI</t>
-  </si>
-  <si>
-    <t>GPS</t>
-  </si>
-  <si>
-    <t>ES</t>
-  </si>
-  <si>
-    <t>JBL</t>
-  </si>
-  <si>
-    <t>CLPT</t>
-  </si>
-  <si>
-    <t>WMB</t>
-  </si>
-  <si>
-    <t>AQN</t>
-  </si>
-  <si>
-    <t>MTN</t>
-  </si>
-  <si>
-    <t>WTRG</t>
-  </si>
-  <si>
-    <t>ARDX</t>
-  </si>
-  <si>
-    <t>KKR</t>
-  </si>
-  <si>
-    <t>IBN</t>
-  </si>
-  <si>
-    <t>AQB</t>
-  </si>
-  <si>
-    <t>SONO</t>
-  </si>
-  <si>
-    <t>NEWR</t>
-  </si>
-  <si>
-    <t>BRKR</t>
-  </si>
-  <si>
-    <t>ITCI</t>
-  </si>
-  <si>
-    <t>CNST</t>
-  </si>
-  <si>
-    <t>HTZGQ</t>
-  </si>
-  <si>
-    <t>SILV</t>
-  </si>
-  <si>
-    <t>CVA</t>
-  </si>
-  <si>
-    <t>RHP</t>
-  </si>
-  <si>
-    <t>NAV</t>
-  </si>
-  <si>
-    <t>JAZZ</t>
-  </si>
-  <si>
-    <t>WEC</t>
-  </si>
-  <si>
-    <t>EVRG</t>
-  </si>
-  <si>
-    <t>AERI</t>
-  </si>
-  <si>
-    <t>UGI</t>
-  </si>
-  <si>
-    <t>MDLA</t>
-  </si>
-  <si>
-    <t>CWK</t>
-  </si>
-  <si>
-    <t>IDCC</t>
-  </si>
-  <si>
-    <t>USAC</t>
-  </si>
-  <si>
-    <t>AGEN</t>
-  </si>
-  <si>
-    <t>ALGM</t>
-  </si>
-  <si>
-    <t>OSH</t>
-  </si>
-  <si>
-    <t>EPZM</t>
-  </si>
-  <si>
-    <t>TROX</t>
-  </si>
-  <si>
-    <t>NS</t>
-  </si>
-  <si>
-    <t>DCI</t>
-  </si>
-  <si>
-    <t>GPMT</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>TMDX</t>
-  </si>
-  <si>
-    <t>GNL</t>
-  </si>
-  <si>
-    <t>QLYS</t>
-  </si>
-  <si>
-    <t>HAE</t>
-  </si>
-  <si>
-    <t>BKEP</t>
-  </si>
-  <si>
-    <t>CKPT</t>
-  </si>
-  <si>
-    <t>BRG</t>
-  </si>
-  <si>
-    <t>CNTY</t>
-  </si>
-  <si>
-    <t>SMSI</t>
-  </si>
-  <si>
-    <t>KIN</t>
-  </si>
-  <si>
-    <t>SMCI</t>
-  </si>
-  <si>
-    <t>ARAV</t>
+    <t>MTEM</t>
+  </si>
+  <si>
+    <t>MDRX</t>
+  </si>
+  <si>
+    <t>ZNTL</t>
+  </si>
+  <si>
+    <t>LAUR</t>
+  </si>
+  <si>
+    <t>PRTK</t>
+  </si>
+  <si>
+    <t>EXTN</t>
+  </si>
+  <si>
+    <t>TSLX</t>
   </si>
   <si>
     <t>CCLP</t>
   </si>
   <si>
-    <t>LCI</t>
-  </si>
-  <si>
-    <t>PLX</t>
-  </si>
-  <si>
-    <t>RBA</t>
-  </si>
-  <si>
-    <t>RADA</t>
-  </si>
-  <si>
-    <t>IEP</t>
-  </si>
-  <si>
-    <t>GRBK</t>
-  </si>
-  <si>
-    <t>BRFS</t>
-  </si>
-  <si>
-    <t>VGR</t>
-  </si>
-  <si>
-    <t>KRMD</t>
-  </si>
-  <si>
-    <t>VOYA</t>
-  </si>
-  <si>
-    <t>WIFI</t>
-  </si>
-  <si>
-    <t>RCM</t>
-  </si>
-  <si>
-    <t>SUPN</t>
-  </si>
-  <si>
-    <t>QTRX</t>
-  </si>
-  <si>
-    <t>JELD</t>
-  </si>
-  <si>
-    <t>SID</t>
-  </si>
-  <si>
-    <t>IPI</t>
-  </si>
-  <si>
-    <t>STIM</t>
-  </si>
-  <si>
-    <t>HALL</t>
-  </si>
-  <si>
-    <t>SMFG</t>
-  </si>
-  <si>
-    <t>MD</t>
-  </si>
-  <si>
-    <t>APTX</t>
-  </si>
-  <si>
-    <t>REKR</t>
-  </si>
-  <si>
-    <t>MBI</t>
-  </si>
-  <si>
-    <t>CBLI</t>
-  </si>
-  <si>
-    <t>MATX</t>
-  </si>
-  <si>
-    <t>UUUU</t>
-  </si>
-  <si>
-    <t>UEC</t>
-  </si>
-  <si>
-    <t>LEAF</t>
-  </si>
-  <si>
-    <t>KYN</t>
-  </si>
-  <si>
-    <t>FNHC</t>
-  </si>
-  <si>
-    <t>EZPW</t>
-  </si>
-  <si>
-    <t>SBBP</t>
-  </si>
-  <si>
-    <t>EVC</t>
-  </si>
-  <si>
-    <t>ETH</t>
-  </si>
-  <si>
-    <t>MTEM</t>
-  </si>
-  <si>
-    <t>MDRX</t>
-  </si>
-  <si>
-    <t>ZNTL</t>
-  </si>
-  <si>
-    <t>LAUR</t>
-  </si>
-  <si>
-    <t>PRTK</t>
-  </si>
-  <si>
-    <t>TSLX</t>
-  </si>
-  <si>
-    <t>EXTN</t>
-  </si>
-  <si>
     <t>SIBN</t>
   </si>
   <si>
@@ -487,69 +475,57 @@
     <t>USAT</t>
   </si>
   <si>
-    <t>$1,509,539.0</t>
+    <t>$1,578,202.5</t>
   </si>
   <si>
     <t>$620,330.0</t>
   </si>
   <si>
-    <t>$345,597.5</t>
-  </si>
-  <si>
-    <t>$323,065.0</t>
-  </si>
-  <si>
-    <t>$294,488.0</t>
+    <t>$402,300.0</t>
+  </si>
+  <si>
+    <t>$256,175.0</t>
   </si>
   <si>
     <t>$174,430.0</t>
   </si>
   <si>
-    <t>$152,709.0</t>
+    <t>$137,470.5</t>
   </si>
   <si>
     <t>$133,725.0</t>
   </si>
   <si>
-    <t>$117,250.0</t>
-  </si>
-  <si>
-    <t>$116,025.0</t>
-  </si>
-  <si>
-    <t>$107,145.0</t>
-  </si>
-  <si>
-    <t>$96,365.0</t>
-  </si>
-  <si>
-    <t>$91,280.0</t>
-  </si>
-  <si>
-    <t>$89,487.5</t>
-  </si>
-  <si>
-    <t>$87,830.0</t>
+    <t>$120,690.0</t>
+  </si>
+  <si>
+    <t>$115,935.0</t>
+  </si>
+  <si>
+    <t>$99,120.0</t>
   </si>
   <si>
     <t>$83,580.0</t>
   </si>
   <si>
-    <t>$80,266.0</t>
+    <t>$81,440.0</t>
   </si>
   <si>
     <t>$77,682.5</t>
   </si>
   <si>
-    <t>$77,624.0</t>
-  </si>
-  <si>
-    <t>$71,180.0</t>
+    <t>$72,705.0</t>
+  </si>
+  <si>
+    <t>$68,264.0</t>
   </si>
   <si>
     <t>$46,538.0</t>
   </si>
   <si>
+    <t>$44,763.0</t>
+  </si>
+  <si>
     <t>$39,360.0</t>
   </si>
   <si>
@@ -559,70 +535,61 @@
     <t>$33,760.0</t>
   </si>
   <si>
-    <t>$33,090.0</t>
-  </si>
-  <si>
     <t>$31,017.5</t>
   </si>
   <si>
     <t>$29,713.0</t>
   </si>
   <si>
-    <t>$27,560.0</t>
-  </si>
-  <si>
-    <t>$26,498.800000000003</t>
-  </si>
-  <si>
-    <t>$25,815.0</t>
-  </si>
-  <si>
-    <t>$23,565.0</t>
-  </si>
-  <si>
-    <t>$22,470.0</t>
+    <t>$26,694.7</t>
+  </si>
+  <si>
+    <t>$23,355.0</t>
   </si>
   <si>
     <t>$21,371.0</t>
   </si>
   <si>
+    <t>$20,071.0</t>
+  </si>
+  <si>
     <t>$19,670.0</t>
   </si>
   <si>
-    <t>$19,617.0</t>
-  </si>
-  <si>
     <t>$17,850.0</t>
   </si>
   <si>
     <t>$15,010.0</t>
   </si>
   <si>
-    <t>$14,552.5</t>
+    <t>$14,999.5</t>
+  </si>
+  <si>
+    <t>$14,569.0</t>
   </si>
   <si>
     <t>$14,331.5</t>
   </si>
   <si>
+    <t>$13,687.5</t>
+  </si>
+  <si>
     <t>$13,649.0</t>
   </si>
   <si>
-    <t>$13,387.5</t>
-  </si>
-  <si>
-    <t>$13,315.0</t>
-  </si>
-  <si>
-    <t>$12,792.5</t>
-  </si>
-  <si>
-    <t>$12,627.5</t>
-  </si>
-  <si>
-    <t>$12,426.0</t>
-  </si>
-  <si>
-    <t>$12,275.5</t>
+    <t>$13,225.0</t>
+  </si>
+  <si>
+    <t>$12,895.0</t>
+  </si>
+  <si>
+    <t>$12,652.5</t>
+  </si>
+  <si>
+    <t>$12,325.0</t>
+  </si>
+  <si>
+    <t>$11,715.0</t>
   </si>
   <si>
     <t>$10,892.5</t>
@@ -637,13 +604,10 @@
     <t>$10,194.0</t>
   </si>
   <si>
-    <t>$9,385.0</t>
-  </si>
-  <si>
     <t>$9,022.5</t>
   </si>
   <si>
-    <t>$8,685.0</t>
+    <t>$8,650.0</t>
   </si>
   <si>
     <t>$8,290.0</t>
@@ -655,9 +619,6 @@
     <t>$7,937.0</t>
   </si>
   <si>
-    <t>$7,930.0</t>
-  </si>
-  <si>
     <t>$7,783.0</t>
   </si>
   <si>
@@ -667,10 +628,19 @@
     <t>$7,470.0</t>
   </si>
   <si>
-    <t>$6,665.0</t>
-  </si>
-  <si>
-    <t>$6,427.5</t>
+    <t>$7,295.0</t>
+  </si>
+  <si>
+    <t>$6,865.0</t>
+  </si>
+  <si>
+    <t>$6,852.5</t>
+  </si>
+  <si>
+    <t>$6,772.5</t>
+  </si>
+  <si>
+    <t>$6,380.0</t>
   </si>
   <si>
     <t>$6,203.0</t>
@@ -679,33 +649,21 @@
     <t>$5,472.0</t>
   </si>
   <si>
-    <t>$5,270.0</t>
-  </si>
-  <si>
     <t>$5,147.5</t>
   </si>
   <si>
     <t>$5,105.0</t>
   </si>
   <si>
-    <t>$4,755.0</t>
-  </si>
-  <si>
     <t>$4,643.0</t>
   </si>
   <si>
-    <t>$4,605.0</t>
-  </si>
-  <si>
     <t>$4,090.0</t>
   </si>
   <si>
     <t>$3,835.0</t>
   </si>
   <si>
-    <t>$3,827.5</t>
-  </si>
-  <si>
     <t>$3,740.0</t>
   </si>
   <si>
@@ -721,7 +679,7 @@
     <t>$3,285.0</t>
   </si>
   <si>
-    <t>$3,182.5</t>
+    <t>$2,882.5</t>
   </si>
   <si>
     <t>$2,765.0</t>
@@ -730,7 +688,10 @@
     <t>$2,665.0</t>
   </si>
   <si>
-    <t>$2,307.5</t>
+    <t>$2,549.0</t>
+  </si>
+  <si>
+    <t>$2,448.0</t>
   </si>
   <si>
     <t>$2,190.0</t>
@@ -739,9 +700,6 @@
     <t>$2,165.0</t>
   </si>
   <si>
-    <t>$2,136.0</t>
-  </si>
-  <si>
     <t>$2,127.5</t>
   </si>
   <si>
@@ -763,6 +721,9 @@
     <t>$1,552.5</t>
   </si>
   <si>
+    <t>$1,505.0</t>
+  </si>
+  <si>
     <t>$1,425.0</t>
   </si>
   <si>
@@ -772,24 +733,21 @@
     <t>$1,385.0</t>
   </si>
   <si>
+    <t>$1,347.5</t>
+  </si>
+  <si>
     <t>$1,335.0</t>
   </si>
   <si>
     <t>$1,325.0</t>
   </si>
   <si>
-    <t>$1,260.0</t>
-  </si>
-  <si>
-    <t>$1,212.5</t>
+    <t>$1,312.5</t>
   </si>
   <si>
     <t>$1,060.0</t>
   </si>
   <si>
-    <t>$995.0</t>
-  </si>
-  <si>
     <t>$984.0</t>
   </si>
   <si>
@@ -802,9 +760,6 @@
     <t>$817.5</t>
   </si>
   <si>
-    <t>$815.0</t>
-  </si>
-  <si>
     <t>$789.0</t>
   </si>
   <si>
@@ -832,9 +787,15 @@
     <t>$550.0</t>
   </si>
   <si>
+    <t>$537.5</t>
+  </si>
+  <si>
     <t>$492.0</t>
   </si>
   <si>
+    <t>$490.0</t>
+  </si>
+  <si>
     <t>$487.5</t>
   </si>
   <si>
@@ -856,27 +817,33 @@
     <t>$400.0</t>
   </si>
   <si>
+    <t>$395.0</t>
+  </si>
+  <si>
     <t>$390.0</t>
   </si>
   <si>
     <t>$387.5</t>
   </si>
   <si>
+    <t>$347.5</t>
+  </si>
+  <si>
     <t>$345.0</t>
   </si>
   <si>
-    <t>$342.5</t>
-  </si>
-  <si>
     <t>$317.5</t>
   </si>
   <si>
+    <t>$307.5</t>
+  </si>
+  <si>
+    <t>$297.5</t>
+  </si>
+  <si>
     <t>$292.0</t>
   </si>
   <si>
-    <t>$257.5</t>
-  </si>
-  <si>
     <t>$170.0</t>
   </si>
   <si>
@@ -905,6 +872,9 @@
   </si>
   <si>
     <t>$102.0</t>
+  </si>
+  <si>
+    <t>$80.0</t>
   </si>
   <si>
     <t>$50.0</t>
@@ -1295,7 +1265,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B156"/>
+  <dimension ref="A1:B152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1314,7 +1284,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1322,7 +1292,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1330,7 +1300,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1338,7 +1308,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1346,7 +1316,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1354,7 +1324,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1362,7 +1332,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1370,7 +1340,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1378,7 +1348,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1386,7 +1356,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1394,7 +1364,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1402,7 +1372,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1410,7 +1380,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1418,7 +1388,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1426,7 +1396,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1434,7 +1404,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1442,7 +1412,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1450,7 +1420,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1458,7 +1428,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1466,7 +1436,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1474,7 +1444,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1482,7 +1452,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1490,7 +1460,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1498,7 +1468,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1506,7 +1476,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1514,7 +1484,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1522,7 +1492,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1530,7 +1500,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1538,7 +1508,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1546,7 +1516,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1554,7 +1524,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1562,7 +1532,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1570,7 +1540,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1578,7 +1548,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1586,7 +1556,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1594,7 +1564,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1602,7 +1572,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1610,7 +1580,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1618,7 +1588,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1626,7 +1596,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1634,7 +1604,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1642,7 +1612,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1650,7 +1620,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1658,7 +1628,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1666,7 +1636,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1674,7 +1644,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1682,7 +1652,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1690,7 +1660,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1698,7 +1668,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1706,7 +1676,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1714,7 +1684,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1722,7 +1692,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1730,7 +1700,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1738,7 +1708,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1746,7 +1716,7 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1754,7 +1724,7 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1762,7 +1732,7 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1770,7 +1740,7 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1778,7 +1748,7 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1786,7 +1756,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1794,7 +1764,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1802,7 +1772,7 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1810,7 +1780,7 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1818,7 +1788,7 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1826,7 +1796,7 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1834,7 +1804,7 @@
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1842,7 +1812,7 @@
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1850,7 +1820,7 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1858,7 +1828,7 @@
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1866,7 +1836,7 @@
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1874,7 +1844,7 @@
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1882,7 +1852,7 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1890,7 +1860,7 @@
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1898,7 +1868,7 @@
         <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1906,7 +1876,7 @@
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1914,7 +1884,7 @@
         <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1922,7 +1892,7 @@
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1930,7 +1900,7 @@
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1938,7 +1908,7 @@
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1946,7 +1916,7 @@
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1954,7 +1924,7 @@
         <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1962,7 +1932,7 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1970,7 +1940,7 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1978,7 +1948,7 @@
         <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1986,7 +1956,7 @@
         <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1994,7 +1964,7 @@
         <v>87</v>
       </c>
       <c r="B87" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -2002,7 +1972,7 @@
         <v>88</v>
       </c>
       <c r="B88" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -2010,7 +1980,7 @@
         <v>89</v>
       </c>
       <c r="B89" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -2018,7 +1988,7 @@
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -2026,7 +1996,7 @@
         <v>91</v>
       </c>
       <c r="B91" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -2034,7 +2004,7 @@
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -2042,7 +2012,7 @@
         <v>93</v>
       </c>
       <c r="B93" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -2050,7 +2020,7 @@
         <v>94</v>
       </c>
       <c r="B94" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -2058,7 +2028,7 @@
         <v>95</v>
       </c>
       <c r="B95" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -2066,7 +2036,7 @@
         <v>96</v>
       </c>
       <c r="B96" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -2074,7 +2044,7 @@
         <v>97</v>
       </c>
       <c r="B97" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -2082,7 +2052,7 @@
         <v>98</v>
       </c>
       <c r="B98" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -2090,7 +2060,7 @@
         <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -2098,7 +2068,7 @@
         <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -2106,7 +2076,7 @@
         <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -2114,7 +2084,7 @@
         <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -2122,7 +2092,7 @@
         <v>103</v>
       </c>
       <c r="B103" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -2130,7 +2100,7 @@
         <v>104</v>
       </c>
       <c r="B104" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -2138,7 +2108,7 @@
         <v>105</v>
       </c>
       <c r="B105" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -2146,7 +2116,7 @@
         <v>106</v>
       </c>
       <c r="B106" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -2154,7 +2124,7 @@
         <v>107</v>
       </c>
       <c r="B107" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -2162,7 +2132,7 @@
         <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -2170,7 +2140,7 @@
         <v>109</v>
       </c>
       <c r="B109" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -2178,7 +2148,7 @@
         <v>110</v>
       </c>
       <c r="B110" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -2186,7 +2156,7 @@
         <v>111</v>
       </c>
       <c r="B111" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -2194,7 +2164,7 @@
         <v>112</v>
       </c>
       <c r="B112" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -2202,7 +2172,7 @@
         <v>113</v>
       </c>
       <c r="B113" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -2210,7 +2180,7 @@
         <v>114</v>
       </c>
       <c r="B114" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -2218,7 +2188,7 @@
         <v>115</v>
       </c>
       <c r="B115" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -2226,7 +2196,7 @@
         <v>116</v>
       </c>
       <c r="B116" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -2234,7 +2204,7 @@
         <v>117</v>
       </c>
       <c r="B117" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -2242,7 +2212,7 @@
         <v>118</v>
       </c>
       <c r="B118" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -2250,7 +2220,7 @@
         <v>119</v>
       </c>
       <c r="B119" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2258,7 +2228,7 @@
         <v>120</v>
       </c>
       <c r="B120" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2266,7 +2236,7 @@
         <v>121</v>
       </c>
       <c r="B121" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2274,7 +2244,7 @@
         <v>122</v>
       </c>
       <c r="B122" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2282,7 +2252,7 @@
         <v>123</v>
       </c>
       <c r="B123" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -2290,7 +2260,7 @@
         <v>124</v>
       </c>
       <c r="B124" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -2298,7 +2268,7 @@
         <v>125</v>
       </c>
       <c r="B125" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -2306,7 +2276,7 @@
         <v>126</v>
       </c>
       <c r="B126" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -2314,7 +2284,7 @@
         <v>127</v>
       </c>
       <c r="B127" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2322,7 +2292,7 @@
         <v>128</v>
       </c>
       <c r="B128" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -2330,7 +2300,7 @@
         <v>129</v>
       </c>
       <c r="B129" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2338,7 +2308,7 @@
         <v>130</v>
       </c>
       <c r="B130" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -2346,7 +2316,7 @@
         <v>131</v>
       </c>
       <c r="B131" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -2354,7 +2324,7 @@
         <v>132</v>
       </c>
       <c r="B132" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -2362,7 +2332,7 @@
         <v>133</v>
       </c>
       <c r="B133" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -2370,7 +2340,7 @@
         <v>134</v>
       </c>
       <c r="B134" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -2378,7 +2348,7 @@
         <v>135</v>
       </c>
       <c r="B135" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -2386,7 +2356,7 @@
         <v>136</v>
       </c>
       <c r="B136" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2394,7 +2364,7 @@
         <v>137</v>
       </c>
       <c r="B137" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2402,7 +2372,7 @@
         <v>138</v>
       </c>
       <c r="B138" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2410,7 +2380,7 @@
         <v>139</v>
       </c>
       <c r="B139" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2418,7 +2388,7 @@
         <v>140</v>
       </c>
       <c r="B140" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2426,7 +2396,7 @@
         <v>141</v>
       </c>
       <c r="B141" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2434,7 +2404,7 @@
         <v>142</v>
       </c>
       <c r="B142" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2442,7 +2412,7 @@
         <v>143</v>
       </c>
       <c r="B143" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2450,7 +2420,7 @@
         <v>144</v>
       </c>
       <c r="B144" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2458,7 +2428,7 @@
         <v>145</v>
       </c>
       <c r="B145" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2466,7 +2436,7 @@
         <v>146</v>
       </c>
       <c r="B146" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -2474,7 +2444,7 @@
         <v>147</v>
       </c>
       <c r="B147" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2482,7 +2452,7 @@
         <v>148</v>
       </c>
       <c r="B148" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2490,7 +2460,7 @@
         <v>149</v>
       </c>
       <c r="B149" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -2498,7 +2468,7 @@
         <v>150</v>
       </c>
       <c r="B150" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -2506,7 +2476,7 @@
         <v>151</v>
       </c>
       <c r="B151" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -2514,39 +2484,7 @@
         <v>152</v>
       </c>
       <c r="B152" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2">
-      <c r="A153" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B153" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2">
-      <c r="A154" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B154" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2">
-      <c r="A155" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B155" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2">
-      <c r="A156" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B156" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>